<commit_message>
New test automation started - Transport tab
</commit_message>
<xml_diff>
--- a/shalmi2/src/main/Shaalmi_Tests.xlsx
+++ b/shalmi2/src/main/Shaalmi_Tests.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\GIT_Repo\shalmi2\src\main\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="252" windowWidth="20112" windowHeight="7812" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Browser" sheetId="5" r:id="rId1"/>
     <sheet name="Registeration_Test" sheetId="1" r:id="rId2"/>
-    <sheet name="Admin_SignIn_Tests" sheetId="2" r:id="rId3"/>
-    <sheet name="LogOut" sheetId="4" r:id="rId4"/>
-    <sheet name="Login_Test" sheetId="6" r:id="rId5"/>
+    <sheet name="Admin_TransportTab_Tests" sheetId="7" r:id="rId3"/>
+    <sheet name="Admin_SignIn_Tests" sheetId="2" r:id="rId4"/>
+    <sheet name="LogOut" sheetId="4" r:id="rId5"/>
+    <sheet name="Login_Test" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
   <si>
     <t>Keyword</t>
   </si>
@@ -29,12 +35,6 @@
     <t>Object type</t>
   </si>
   <si>
-    <t>GO2URL</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
@@ -102,12 +102,21 @@
   </si>
   <si>
     <t>CLEANTEXT</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>XPATH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,6 +201,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -239,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,9 +284,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,6 +336,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -489,16 +535,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -509,21 +555,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,17 +580,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -555,21 +591,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,70 +615,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -652,20 +649,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,32 +674,70 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -710,21 +746,79 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,217 +829,217 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>